<commit_message>
Added login and post ad Title test cases
</commit_message>
<xml_diff>
--- a/src/main/java/co/selenium/framework/TestData/LoginTestData.xlsx
+++ b/src/main/java/co/selenium/framework/TestData/LoginTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSwami\Pro_Kijiji\src\main\java\co\selenium\framework\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView activeTab="1" windowHeight="12300" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="LoginData" r:id="rId2" sheetId="1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+  <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Password</t>
   </si>
@@ -62,17 +67,14 @@
   </si>
   <si>
     <t>Welcome@001</t>
-  </si>
-  <si>
-    <t>TC_Login_02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,14 +437,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
@@ -451,7 +453,7 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="16.5" r="1" spans="1:5" thickBot="1" thickTop="1">
+    <row ht="16.5" r="1" spans="1:5" thickBot="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -468,7 +470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:5" thickTop="1">
+    <row ht="15.75" r="2" spans="1:5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -496,14 +498,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
@@ -511,7 +513,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="16.5" r="1" spans="1:4" thickBot="1" thickTop="1">
+    <row ht="16.5" r="1" spans="1:4" thickBot="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -525,7 +527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:4" thickTop="1">
+    <row ht="15.75" r="2" spans="1:4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -537,11 +539,6 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>